<commit_message>
TME develop V8 more articles auto add type in database
</commit_message>
<xml_diff>
--- a/productdata.xlsx
+++ b/productdata.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="12645" windowWidth="22260" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -54,12 +54,11 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle builtinId="0" name="Обычный" xfId="0"/>
@@ -324,7 +323,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -336,1137 +335,1890 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L1048576"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="16.28515625"/>
-    <col customWidth="1" max="2" min="2" width="12.5703125"/>
-    <col customWidth="1" max="3" min="3" width="23.85546875"/>
+    <col customWidth="1" max="1" min="1" style="2" width="16.28515625"/>
+    <col customWidth="1" max="2" min="2" style="2" width="12.5703125"/>
+    <col customWidth="1" max="3" min="3" style="2" width="23.85546875"/>
+    <col customWidth="1" max="7" min="7" style="3" width="9.140625"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
-        <is>
-          <t>09-50-3021</t>
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>1N4007-DC</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>MX-2139-2A</t>
+          <t>1N4007-DC</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Вилка; провод-плата; "мама"; KK 396; 3,96мм; PIN: 2; без контактов</t>
+          <t>Диод: выпрямительный; THT; 1кВ; 1А; Упаковка: Ammo Pack; DO41</t>
         </is>
       </c>
       <c r="D1" t="n">
-        <v>0.00053</v>
+        <v>0.00028</v>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>static.tme.eu/products_pics/a/d/c/adc7a7c41eb9a5687179d7eef91a53a8/338104.jpg</t>
+          <t>static.tme.eu/products_pics/f/c/8/fc82c3993bd1e575e9e7935e29e432c3/56940.jpg</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>www.tme.eu/ru/details/mx-2139-2a/razemy-signalnye-rastr-3-96mm/molex/09-50-3021/</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>{'Производитель': 'MOLEX', '#Promotion': 'africa_anniversary', 'Разъем': 'вилка', 'Тип разъема': 'провод - плата', 'Вид разъемов': '"мама"', 'Серия разъема': 'KK 396', 'Шаг контактов': '3,96мм', 'Кол-во выводов': '2', 'Версия разъема': 'без контактов', 'Механический монтаж': 'на провод', 'Класс горючести': 'UL94V-2', 'Конфигурация выводов разъема': '1x2', 'Рабочее напряжение макс.': '250В', 'Дополнительная информация': 'больше товаров данной серии доступно на www.tme.eu', 'Alias': '9503021', 'Engineering PN': '2139-2A'}</t>
+          <t>www.tme.eu/ru/details/1n4007-dc/universalnye-diody-tht/dc-components/1n4007/</t>
+        </is>
+      </c>
+      <c r="G1" s="3" t="inlineStr">
+        <is>
+          <t>{'Тип диода': 'выпрямительный', 'Монтаж': 'THT', 'Обратное напряжение макс.': '1кВ', 'Прямой ток': '1А', 'Конструкция диода': 'одиночный диод', 'Вид упаковки': 'Ammo Pack', 'Корпус': 'DO41', 'Импульсный ток': '30А', 'Падение напряжения макс.': '1,1В'}</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>www.tme.eu/Document/c553b43254396d60e30fc0ad52ecb64e/9503101.pdf</t>
+          <t>www.tme.eu/Document/b9a3e8c499478bdb2cb9098c529c9361/1N4001_ser.pdf</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t>VTP4085H</t>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>NE555D</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>VTP4085H</t>
+          <t>NE555D</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Фотодиод; 925нм; 400-1100нм; Монтаж: THT; 100нА</t>
+          <t>Периферийная микросхема; нестабильный,моностабильная,часы RC</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.000603</v>
+        <v>6.7e-05</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>static.tme.eu/products_pics/5/2/7/5272851219b4bcbf50385c044b80ce2c/361407.jpg</t>
+          <t>static.tme.eu/products_pics/4/8/a/48a33ccfb5a851d5982dcdda0776f7ac/285338.jpg</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>www.tme.eu/ru/details/vtp4085h/fotodiody/excelitas/</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>{'Производитель': 'Excelitas', 'Тип фотоприемника': 'фотодиод', 'Длина волны в точке макс. чувствительности': '925нм', 'Длина волны λd': '400-1100нм', 'Светочувствительная поверхность': '21мм&lt;sup&gt;2&lt;/sup&gt;', 'Монтаж': 'THT', 'Темновой ток': '100нА', '#Common #name - #search': 'perkin elmer'}</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>www.tme.eu/Document/7e50f44c383244e46c42b0ac55270bde/3.pdf</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="30" r="3">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>PMD1238PKB1-A.(2).F.GN</t>
+          <t>www.tme.eu/ru/details/ne555d/mikroskhemy-watchdog-i-reset/texas-instruments/</t>
+        </is>
+      </c>
+      <c r="G2" s="3" t="inlineStr">
+        <is>
+          <t>{'Тип микросхемы': 'периферийная микросхема', 'Вид микросхемы': 'часы RC', 'Частота': '500кГц', 'Напряжение питания': '4,5...16В DC', 'Корпус': 'SO8', 'Ток питания DC': '10мА', 'Монтаж': 'SMD', 'Рабочая температура': '0...70°C', 'Вид упаковки': 'туба', 'Кол-во каналов': '1'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>VUM24-05N</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>PMD1238PKB1AF</t>
+          <t>VUM24-05N</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Вентилятор: DC; осевой; 12ВDC; 38x38x20мм; 20,39м3/ч; 44дБА; 26AWG</t>
+          <t>Модуль; диод/транзистор; 500В; 24А; V1-B-Pack; Ugs: ±20В; винтами</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0.0286</v>
+        <v>0.0471</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>static.tme.eu/products_pics/3/d/b/3dbb5a0071d20d3ee13a7810da56ffd9/423955.jpg</t>
+          <t>static.tme.eu/products_pics/0/2/2/0220bb819b9637a92649c24ad14225f6/408702.jpg</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>www.tme.eu/ru/details/pmd1238pkb1af/ventiliatory-dc-12v/sunon/pmd1238pkb1-a-2-f-gn/</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>{'Производитель': 'SUNON', 'Тип вентилятора': 'DC', 'Вид вентилятора': 'осевой', 'Напряжение питания': '12В DC', 'Размер вентилятора': '38x38x20мм', 'Потребл. мощность': '3,1Вт', 'Номинальный ток': '0,26А', 'Воздушный поток': '20,39м&lt;sup&gt;3&lt;/sup&gt;/ч', 'Уровень шума': '44дБА', 'Вид подшипника': 'шариковый', 'Сигнальный вывод': 'Типа F', 'Скорость вращения': '13000 (±10%)об./мин.', 'Вес': '27г', 'Отклонение потребляемой мощности и тока': '±15%', 'Сопротивление изоляции мин.': '10МОм', 'Материал крыльчатки': 'термопласт', 'Материал корпуса': 'термопласт', 'Класс изоляции': 'E', 'Выводы': '3 провода', 'Рабочая температура': '-10...70°C', 'Длина провода': '300мм', 'Статическое давление': '15,49мм H&lt;sub&gt;2&lt;/sub&gt;O', 'Мотор вентилятора': 'бесколлекторный, DC', 'Класс горючести': 'UL94V-0', '#Promotion': 'africa_anniversary', 'Дополнительные функции': 'автоперезапуск', 'Рабочее напряжение': '6...13,8В', 'Размер провода': '26AWG'}</t>
+          <t>www.tme.eu/ru/details/vum24-05n/tranzistornye-moduli-mosfet/ixys/</t>
+        </is>
+      </c>
+      <c r="G3" s="3" t="inlineStr">
+        <is>
+          <t>{'Тип модуля': 'транзисторный', 'Конструкция диода': 'диод/транзистор', 'Напряжение сток-исток': '500В', 'Ток стока': '24А', 'Корпус': 'V1-B-Pack', 'Топология': 'тормозной транзистор', 'Монтаж': 'винтами', 'Электрический монтаж': 'коннекторы FASTON', 'Сопротивление в открытом состоянии': '120мОм', 'Ток стока в импульсном режиме': '95А', 'Рассеиваемая мощность': '170Вт', 'Заряд затвора': '350нC', 'Напряжение затвор-исток': '±20В'}</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>www.tme.eu/Document/78a82a4c563b234694f3bba2d3281ea2/High_Air_Flow_Series_e_2012.pdf</t>
+          <t>www.tme.eu/Document/fd7f4c65604a52c1c2e7050eec874898/VUM24-05N.pdf</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>SR17A1620F69N</t>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>OPT-LY-04FL</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>SR17A1620F69N</t>
+          <t>OPT-LY04FL</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Переключатель: поворотный; Положения: 6; 0,3A/16ВDC; 30°; -20÷70°C</t>
+          <t>Инструмент: для опрессовки; 0,5÷1мм2; 20AWG÷18AWG</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.00728</v>
+        <v>0.5699</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>static.tme.eu/products_pics/4/f/4/4f4c3b24c14c9b50fb37d0442c936216/463798.jpg</t>
+          <t>static.tme.eu/products_pics/6/7/3/673972bba7e2b96d74e24df76fb4a91c/471986.jpg</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>www.tme.eu/ru/details/sr17a1620f69n/perekliuchateli-oborotnye/ninigi/</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>{'Производитель': 'NINIGI', 'Тип переключателя': 'поворотный', 'Количество возможных положений': '6', 'Нагрузка контакта DC @R': '0,3A / 16В DC', 'Кол-во секций': '1', 'Угол поворота на позицию': '30°', 'Рабочая температура': '-20...70°C', 'Выводы': 'прямые', 'Алгоритм работы': 'BBM (non-shorting)', 'Материал контакта': 'латунь', '#Promotion': 'africa_anniversary', 'Сопротивление контакта макс.': '50мОм', 'Материал корпуса': 'сталь', 'Ресурс': '10000циклов', 'Сопротивление изоляции мин.': '100МОм', 'Вид оси': 'гладкая', 'Диаметр оси': '6мм', 'Длина оси': '12мм', 'Монтажная резьба': 'M9x0,75', 'Момент вращения': '2,9Нсм', 'Кол-во фиксированных положений': '6'}</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>www.tme.eu/Document/88b118568280ff5ee439306dcb657dd4/SR17A1620F69N_DRAWING.pdf</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="30" r="5">
-      <c r="A5" s="2" t="inlineStr">
-        <is>
-          <t>VLMW41R1T1-7K8L-08</t>
+          <t>www.tme.eu/ru/details/opt-ly04fl/zazhimnye-ust-va-kabelnykh-nakonechnikov/opt/opt-ly-04fl/</t>
+        </is>
+      </c>
+      <c r="G4" s="3" t="inlineStr">
+        <is>
+          <t>{'Тип инструмента': 'для опрессовки', 'Назначение инструмента': 'угловые кабельные наконечники 90° без изоляции', 'Сечение провода': '0,5...1мм&lt;sup&gt;2&lt;/sup&gt;', 'Размер провода': '20AWG...18AWG'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>GSM90A12-P1M</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>VLMW41R1T1-7K8L-08</t>
+          <t>GSM90A12-P1M</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>LED; SMD; 3528,PLCC2; белый холодный; 112÷355мкд; 5000(тип.)K</t>
+          <t>Блок питания: импульсный; 12ВDC; 6,67А; Вых: 5,5/2,5; 80Вт; 88%</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>9.6e-05</v>
+        <v>0.4637</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>static.tme.eu/products_pics/b/6/b/b6bd106244234a961251c16ee584774e/492739.jpg</t>
+          <t>static.tme.eu/products_pics/e/a/2/ea24e9403a74f9a1338252945f89309a/464883.jpg</t>
         </is>
       </c>
       <c r="F5" s="1" t="inlineStr">
         <is>
-          <t>www.tme.eu/ru/details/vlmw41r1t1-7k8l-08/svetodiody-smd-belye/vishay/</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>{'Производитель': 'VISHAY', 'Тип диода': 'LED', 'Монтаж': 'SMD', 'Корпус': 'PLCC2', 'Цвет диодa LED': 'белый холодный', 'Сила света': '112...355мкд', 'Цветовая температура': '5000 (тип.)K', 'Размеры': '3,5x2,8x1,75мм', '#Promotion': 'blackpool18', 'Ток диода LED': '10мА', 'Поверхность': 'плоская', 'Рабочее напряжение': '3,3...4,2В', 'Обзор': '120°'}</t>
+          <t>www.tme.eu/ru/details/gsm90a12-p1m/bloki-pitaniia-nastolnye/mean-well/</t>
+        </is>
+      </c>
+      <c r="G5" s="3" t="inlineStr">
+        <is>
+          <t>{'Тип блока питания': 'импульсный', 'Ток выхода макс.': '6,67А', 'Вид выходного разъема': '5,5/2,5', 'Мощность': '80Вт', 'Вид корпуса': 'настольный', 'Вид блока питания': 'стабилизатор напряжения', 'Состав набора': 'без шнура питания', 'Длина выходного провода': '1м', 'Внешние размеры': '145x60x32мм', 'Рабочая температура': '-30...70°C', 'Защита': 'от перенапряжения', '#Common #name - #search': 'настольный', 'Соответствуют норме': 'Energy efficiency Level VI', 'Вид входного разъема': 'IEC C14', 'Версия разъема': 'прямой', 'КПД': '88%', 'Полярность': 'плюс в центре', 'Напряжение питания': '113...370В DC', 'Применение': 'медицинская аппаратура', 'Выходное напряжение': '12В DC'}</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>www.tme.eu/Document/25492a798f338a61c91ed67f6fe64428/VLMW41R1T1-7K8L-08-DTE.pdf</t>
+          <t>www.tme.eu/Document/a49b9e6dd8f7f0fcd9388f7568b190e4/INB-MN-ADAPTOR-RU.pdf</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="inlineStr">
-        <is>
-          <t>KG-016</t>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>PREMIUM 111 19MMX20M BLACK</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>KG-016</t>
+          <t>PLH-P111-19-20/BK</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Защитная кромка; полиэтилен; L: 10м; натуральный; H: 5,2мм; W: 4,5мм</t>
+          <t>Лента: электроизоляционная; W: 19мм; L: 20м; D: 0,18мм; черный; 260%</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.153</v>
+        <v>0.09279999999999999</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>static.tme.eu/products_pics/8/e/b/8eb8e34502421cab59eaac4e2125b4b1/28137.jpg</t>
+          <t>static.tme.eu/products_pics/6/8/2/68240fc5a5888f45ed2accb44ffde5c0/612586.jpg</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>www.tme.eu/ru/details/kg-016/zashchitnye-nasadki-na-kraia/fix-fasten/</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>{'Производитель': 'FIX&amp;FASTEN', 'Тип аксессуаров для корпусов': 'защитная кромка', 'Материал корпуса': 'полиэтилен', 'Длина': '10м', 'Цвет': 'натуральный', 'Высота': '5,2мм', 'Ширина': '4,5мм', 'Толщина панели': '1,45...1,75мм', 'Версия': 'с надрезами'}</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>www.tme.eu/Document/eada3f842acb4e4fa3a63ef1cbb6d29f/KG-010.pdf</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="30" r="7">
-      <c r="A7" s="2" t="inlineStr">
-        <is>
-          <t>SKIIP 23NAB126V1 M20</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>SKIIP23NAB126V1</t>
+          <t>www.tme.eu/ru/details/plh-p111-19-20_bk/lenty-izoliatsionnye/plymouth/premium-111-19mmx20m-black/</t>
+        </is>
+      </c>
+      <c r="G6" s="3" t="inlineStr">
+        <is>
+          <t>{'Тип ленты': 'электроизоляционная', 'Ширина': '19мм', 'Длина': '20м', 'Толщина': '0,18мм', 'Цвет': 'черный', 'Вид клея': 'каучуковый', 'Материал носителя': 'пленка ПВХ', 'Применение ленты': 'изоляция электрических проводов и кабелей', 'Рабочая температура': '-10...105°C', 'Удлинение при разрыве': '260%', 'Адгезия к стали': '2,2Н/cм', 'Характеристики лент': 'эластичная', 'Устойчивы к': 'УФ-излучению', 'Диэлектрическая прочность': '8кВ'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>ЖОПА</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Модуль: IGBT; диод/транзистор; 3-фазный мост IGBT; Urmax: 1,2кВ</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>0.058</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>static.tme.eu/products_pics/b/8/8/b88b516c6fd7e20a7f255335f0fd83ea/672271.jpg</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>www.tme.eu/ru/details/skiip23nab126v1/moduli-igbt/semikron/skiip-23nab126v1-m20/</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>{'Производитель': 'SEMIKRON', 'Тип модуля': 'IGBT', 'Конструкция диода': 'диод/транзистор', 'Топология': 'тормозной транзистор', 'Обратное напряжение макс.': '1,2кВ', 'Ток коллектора': '31А', 'Мощность': '7,5кВт', 'Корпус': 'MiniSKiiP® 2', 'Применение': 'преобразователь частоты', 'Электрический монтаж': 'Press-Fit', 'Монтаж': 'винтами', 'Напряжение затвор - эмиттер': '±20В', 'Ток коллектора в импульсе': '50А'}</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>www.tme.eu/Document/1cb1fd4f4f1b21d6215cc105030095bf/SKiiP23NAB126V1.pdf</t>
+          <t>Артикула нет на TME</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="inlineStr">
-        <is>
-          <t>SCP-50-12</t>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>VLMW1500-GS08</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>SCP-50-12</t>
+          <t>VLMW1500-GS08</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Блок питания: ИБП; модульный; 49,7Вт; 13,8ВDC; 129x98x38мм; 3,6А</t>
+          <t>LED; SMD; 0402; белый; 45÷180мкд; 65°; 5мА; 2,65÷3,05В</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.4291</v>
+        <v>0.0001</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>static.tme.eu/products_pics/e/8/4/e846528474d9805d9a18c058c84e8d02/206779.jpg</t>
+          <t>static.tme.eu/products_pics/3/5/0/35030a3c2879da88a43558958b1e6a69/520930.jpg</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>www.tme.eu/ru/details/scp-50-12/bloki-pitaniia-dlia-vstraivaniia/mean-well/</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>{'Производитель': 'MEAN WELL', 'Тип блока питания': 'ИБП', 'Вид блока питания': 'модульный', 'Мощность': '49,7Вт', 'Внешние размеры': '129x98x38мм', 'Выходной ток': '3,6А', 'Характеристики блоков питания/преобразователей': 'номинальные параметры при полной нагрузке', 'Вес': '450г', 'Рабочая температура': '-20...60°C', 'Количество выходов': '1', 'Электрическое подключение': 'клеммная колодка', 'Монтаж': 'открытое исполнение', 'Защита': 'от увеличения напряжения', 'Напряжение питания': '120...370В DC', '#Promotion': 'automatics-components_promo', 'КПД': '81%', 'Вид корпуса': '903', 'Сопутствующие товары': 'DRP-03', 'Выходное напряжение': '13,8В DC'}</t>
+          <t>www.tme.eu/ru/details/vlmw1500-gs08/svetodiody-smd-belye/vishay/</t>
+        </is>
+      </c>
+      <c r="G8" s="3" t="inlineStr">
+        <is>
+          <t>{'Тип диода': 'LED', 'Монтаж': 'SMD', 'Корпус': '0402', 'Цвет диодa LED': 'белый', 'Сила света': '45...180мкд', 'Размеры': '1x0,5x0,35мм', 'Ток диода LED': '5мА', 'Хроматические координаты': 'x: 0.304; y: 0.3', 'Поверхность': 'плоская', 'Рабочее напряжение': '2,65...3,05В', 'Обзор': '65°'}</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>www.tme.eu/Document/c6ad60a54b368fbe5896a4446dd99732/INB-ZAS-IMP-RU.pdf</t>
+          <t>www.tme.eu/Document/71274733fa94e88759ee47d48ff148f8/VLMW1500-GS08.pdf</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="2" t="inlineStr">
-        <is>
-          <t>ALTIMU-10 V5</t>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>HSG-70-48</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>POLOLU-2739</t>
+          <t>HSG-70-48</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Датчик: положения; 2,5÷5,5ВDC; I2C; LIS3MDL,LPS25H,LSM6DS33</t>
+          <t>Блок питания: импульсный; LED; 72Вт; 48ВDC; 0,9÷1,5А; 90÷305ВAC</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.00253</v>
+        <v>0.802</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>static.tme.eu/products_pics/a/9/b/a9b2dd2c060afe3a66e9976681f00b71/564792.jpg</t>
+          <t>static.tme.eu/products_pics/d/6/9/d695de26f7564e2c2670645117bb948f/340943.jpg</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>www.tme.eu/ru/details/pololu-2739/datchiki-polozheniia/pololu/altimu-10-v5/</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>{'Производитель': 'POLOLU', '#Promotion': 'holidays_201812', '#Common #name - #search': 'модуль', 'Тип датчика': 'положения', 'Вид датчика': 'цифровой компас', 'Напряжение питания': '2,5...5,5В DC', 'Интерфейс': 'I2C', 'Микросхема': 'LSM6DS33', 'Диапазон измерения акселерометра': '±2, ±4, ±8, ±16g', 'Состав набора': 'разъемы', 'Диапазон измерения гироскопа': '±125, ±245, ±500, ±1000, ±2000°/с', 'Диапазон измерения магнетометра': '±4, ±8, ±12, ±16Гс', 'Дополнительные функции': 'регулятор напряжения', 'Диапазон измерения барометра': '26кПа...126кПа', 'Информация': 'Товар не являтся готовым устройством, а лишь его компонентом'}</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="30" r="10">
-      <c r="A10" s="2" t="inlineStr">
-        <is>
-          <t>RTM-5021-CHROM</t>
+          <t>www.tme.eu/ru/details/hsg-70-48/bloki-pitaniia-dlia-led/mean-well/</t>
+        </is>
+      </c>
+      <c r="G9" s="3" t="inlineStr">
+        <is>
+          <t>{'Тип блока питания': 'импульсный', 'Применение': 'LED', 'Вид блока питания': 'CV+CC', 'Мощность': '72Вт', 'Выходное напряжение': '48В DC', 'Выходной ток': '0,9...1,5А', 'Напряжение питания': '127...431В DC', 'Класс защиты': 'IP65', 'Внешние размеры': '127,2x90x38,8мм', 'Характеристики блоков питания/преобразователей': 'номинальные параметры при полной нагрузке', 'Защита': 'от увеличения напряжения', 'Вес': '760г', 'Рабочая температура': '-40...70°C', 'Электрическое подключение': 'провода 300мм', 'Количество выходов': '1', 'Дополнительные функции': 'регулировка выходного тока', 'Серия': 'HSG-70', 'КПД': '90%'}</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>www.tme.eu/Document/8f6b9eb035fb2946c20da9fe547dba90/INB-MN-LED-RU.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>RID-125-1224</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>RTM-5021-CHROM</t>
+          <t>RID-125-1224</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Держатель LED; 5мм; хром; вогнутый; с резиновой заглушкой</t>
+          <t>Блок питания: импульсный; модульный; 133,2Вт; 12ВDC; 199x98x38мм</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.0035</v>
+        <v>0.6371</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>static.tme.eu/products_pics/3/b/f/3bf746acf7bafb655ac88faefb1b5461/374462.jpg</t>
+          <t>static.tme.eu/products_pics/e/7/f/e7fb06cddaa35adfeca9afd3924affcb/303747.jpg</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>www.tme.eu/ru/details/rtm-5021-chrom/patrony/</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>{'Тип аксессуаров для диодов LED': 'держатель LED', 'Диаметр диода LED': '5мм', 'Материал покрытия': 'хром', 'Вид держателя LED': 'вогнутый', 'Версия держателя': 'с резиновой заглушкой', 'Диаметр монтажного отверстия': '8,2мм', '#Promotion': 'blackpool18'}</t>
+          <t>www.tme.eu/ru/details/rid-125-1224/bloki-pitaniia-dlia-vstraivaniia/mean-well/</t>
+        </is>
+      </c>
+      <c r="G10" s="3" t="inlineStr">
+        <is>
+          <t>{'Тип блока питания': 'импульсный', 'Вид блока питания': 'модульный', 'Мощность': '133,2Вт', 'Внешние размеры': '199x98x38мм', 'Выходное напряжение 2': '24В DC', 'Выходной ток': '3,7 (1...7)А', 'Ток на выходе 2': '3,7 (0,4...5)А', 'Характеристики блоков питания/преобразователей': 'изолированный выход и заземление', 'Вес': '700г', 'Рабочая температура': '-25...70°C', 'Количество выходов': '2', 'Электрическое подключение': 'клеммная колодка', 'Монтаж': 'открытое исполнение', 'Защита': 'от увеличения напряжения', 'Напряжение питания': '248...373В DC', 'КПД': '85%', 'Серия': 'RID-125', 'Вид корпуса': '902A', 'Выходное напряжение': '12В DC'}</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>www.tme.eu/Document/ee6f0e6a23c81f0c481af689425f21b2/INB-MN-ENCLOSED-RU.pdf</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="2" t="inlineStr">
-        <is>
-          <t>ULQ2803A</t>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>RG240128B-BIW-V</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>ULQ2803A</t>
+          <t>RG240128B-BIW-V</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Driver; darlington,транзисторная матрица; 0,5А; 50В; Каналы: 8</t>
+          <t>Дисплей: LCD; графический; 240x128; STN Negative; голубой; LED</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.00124</v>
+        <v>0.1835</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>static.tme.eu/products_pics/3/0/d/30d53284f17bcf109c5d334b1dbb0727/285539.jpg</t>
+          <t>static.tme.eu/products_pics/c/1/4/c14588a6b4dd8aea0ea73bd09f497a52/444422.jpg</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>www.tme.eu/ru/details/ulq2803a/draivery-mikroskhemy/stmicroelectronics/</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>{'Производитель': 'STMicroelectronics', 'Тип микросхемы': 'driver', 'Вид микросхемы': 'транзисторная матрица', 'Выходной ток': '0,5А', 'Выходное напряжение': '50В', 'Кол-во каналов': '8', 'Монтаж': 'THT', 'Рабочая температура': '-40...105°C', 'Входное напряжение': '30В', 'Корпус': 'DIP18'}</t>
+          <t>www.tme.eu/ru/details/rg240128b-biw-v/displei-lcd-graficheskie/raystar-optronics/</t>
+        </is>
+      </c>
+      <c r="G11" s="3" t="inlineStr">
+        <is>
+          <t>{'Тип дисплея': 'LCD', 'Вид дисплея': 'графический', 'Разрешение матрицы': '240x128', 'Технология индикатора': 'STN Negative', 'Цвет фона': 'голубой', 'Размеры': '144x104x14,3мм', 'Размер окна (выс. х шир.)': '114x64мм', 'Подсветка': 'LED', 'Цвет подсветки': 'белый', 'Вид контроллера': 'RA6963', 'Кол-во выводов': '20', 'Конфигурация выводов разъема': '1x20', 'Напряжение питания': '3...5,5В DC', 'Шаг контактов': '2,54мм'}</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>www.tme.eu/Document/2e00ebb85c11ad4f6f7cfcae7e101143/ulq2803.pdf</t>
+          <t>www.tme.eu/Document/fd0f5c08ed6f8621c0f022007942f58e/RG240128B-BIW-V.pdf</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="2" t="inlineStr">
-        <is>
-          <t>WDR-480-48</t>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>HAC0251S4-000U-999</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>WDR-480-48</t>
+          <t>HAC0251S4</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Блок питания: импульсный; 480Вт; 48ВDC; 48÷55ВDC; 10А; 180÷550ВAC</t>
+          <t>Вентилятор: DC; осевой; 12ВDC; 120x120x25мм; 93,5м3/ч; 29,6дБА</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>1.649</v>
+        <v>0.1007</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>static.tme.eu/products_pics/3/3/c/33c3235af96f4db2c8837262c86fe4fc/375150.jpg</t>
+          <t>static.tme.eu/products_pics/1/c/4/1c4f6493899f3d28da59a97ab5c64830/413886.jpg</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>www.tme.eu/ru/details/wdr-480-48/bloki-pitaniia-na-din-reiku/mean-well/</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>{'Производитель': 'MEAN WELL', 'Тип блока питания': 'импульсный', 'Мощность': '480Вт', 'Выходной ток': '10А', 'Напряжение питания': '254...780В DC', 'Электрическое подключение': 'клеммная колодка', 'Монтаж': 'DIN', 'Внешние размеры': '85,5x125,2x128,5мм', 'Вес': '1,7кг', 'Количество выходов': '1', 'Рабочая температура': '-30...70°C', 'Защита': 'перенапряжения', 'КПД': '93%', 'Дополнительные функции': 'сигнализация корректного выходного напряжения (контакт NO)', 'Характеристики блоков питания/преобразователей': 'номинальные параметры при полной нагрузке', '#Promotion': 'automatics-components_promo', 'Серия': 'WDR-480', 'Вид корпуса': '984B', 'Выходное напряжение': '48...55В DC'}</t>
+          <t>www.tme.eu/ru/details/hac0251s4/ventiliatory-dc-12v/sunon/hac0251s4-000u-999/</t>
+        </is>
+      </c>
+      <c r="G12" s="3" t="inlineStr">
+        <is>
+          <t>{'Тип вентилятора': 'DC', 'Вид вентилятора': 'осевой', 'Напряжение питания': '12В DC', 'Размер вентилятора': '120x120x25мм', 'Потребл. мощность': '1,9Вт', 'Номинальный ток': '0,155А', 'Воздушный поток': '93,5м&lt;sup&gt;3&lt;/sup&gt;/ч', 'Уровень шума': '29,6дБА', 'Вид подшипника': 'скольжения', 'Скорость вращения': '1600 (±10%)об./мин.', 'Вес': '99г', 'Отклонение потребляемой мощности и тока': '±15%', 'Сопротивление изоляции мин.': '10МОм', 'Материал крыльчатки': 'термопласт', 'Материал корпуса': 'термопласт', 'Класс изоляции': 'A', 'Выводы': '2 провода', 'Рабочая температура': '-10...70°C', 'Длина провода': '330мм', 'Статическое давление': '1,52мм H&lt;sub&gt;2&lt;/sub&gt;O', 'Мотор вентилятора': 'бесколлекторный, DC', 'Класс горючести': 'UL94V-0', 'Рабочее напряжение': '4,5...13,8В', 'Размер провода': '28AWG'}</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>www.tme.eu/Document/72fc6877a395baae40163dbe9cc3995a/INB-ZAS-DIN-RU.pdf</t>
+          <t>www.tme.eu/Document/623c5d7e83fdbabf901aec520d1bc17a/HA_Series.pdf</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="2" t="inlineStr">
-        <is>
-          <t>SF68G</t>
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>PT6KV502A2020</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>SF68G-YAN</t>
+          <t>PT6LV-5K</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Диод: выпрямительный; THT; 600В; 6А; Упаковка: лента; R6; 35нс</t>
+          <t>Потенциометр: монтажный; однооборотный,горизонтальный; 5кОм</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.0019</v>
+        <v>0.000202</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>static.tme.eu/products_pics/a/6/6/a66bd3e70b210db4edb54b4b58c697fb/550499.jpg</t>
+          <t>static.tme.eu/products_pics/e/f/7/ef7e00e5d533007f5b811e74d2cc6779/607737.jpg</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>www.tme.eu/ru/details/sf68g-yan/universalnye-diody-tht/yangjie-technology/sf68g/</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>{'Производитель': 'YANGJIE TECHNOLOGY', 'Тип диода': 'выпрямительный', 'Монтаж': 'THT', 'Обратное напряжение макс.': '600В', 'Прямой ток': '6А', 'Конструкция диода': 'одиночный диод', 'Характеристики полупроводниковых элементов': 'супер-быстрое переключение', 'Вид упаковки': 'лента', 'Корпус': 'R6', 'Время готовности': '35нс', 'Импульсный ток': '150А', 'Падение напряжения макс.': '1,7В'}</t>
+          <t>www.tme.eu/ru/details/pt6lv-5k/potentsiometry-tht-odnooborotnye/piher/pt6kv502a2020/</t>
+        </is>
+      </c>
+      <c r="G13" s="3" t="inlineStr">
+        <is>
+          <t>{'Тип потенциометра': 'монтажный', 'Вид потенциометра': 'однооборотный', 'Сопротивление': '5кОм', 'Мощность': '100мВт', 'Погрешность': '±20%', 'Характеристика': 'линейная', 'Серия потенциометров': 'PT6LV', 'Стандарт потенциометра': '6мм', 'Угол поворота механический': '235 ±5°', 'Крутящий момент': '0,2...2Нсм', 'Рабочее напряжение макс.': '100В', 'Рабочая температура': '-25...70°C', 'Монтаж': 'THT', 'Шаг выводов': '5x5мм', 'Материал дорожки': 'углеродистый', 'Угол поворота электрический': '220 ±20°', 'Размеры корпуса': 'Ø6,3x3,3мм'}</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>www.tme.eu/Document/3084130a016246a43a5d85e56be18eaf/SF61G_SER.pdf</t>
+          <t>www.tme.eu/Document/7ad208364d9e5b91e65e440c0e9c3442/PT6Lx.pdf</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="2" t="inlineStr">
-        <is>
-          <t>SFH 4645</t>
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>PR185-100R-A-16P6</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>SFH4645</t>
+          <t>PR185-100R-A-P6</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>ИК-передатчик; 940нм; прозрачная; 80мВт; 15°; SMD; 100мА; 1,5÷1,8В</t>
+          <t>Потенциометр: осевой; 100Ом; 200мВт; ±20%; под пайку; 6мм; L: 16мм</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>2e-05</v>
+        <v>0.00695</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>static.tme.eu/products_pics/b/f/0/bf06162c05a27b0624acf3a34115a6d9/586741.jpg</t>
+          <t>static.tme.eu/products_pics/0/d/2/0d2b6e5b5f0e4998699f6974d3c1a06b/287262.jpg</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>www.tme.eu/ru/details/sfh4645/infrakrasnye-ledy/osram/sfh-4645/</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>{'Производитель': 'OSRAM', 'Тип диода': 'ИК-передатчик', 'Длина волны λp': '940нм', 'Линза диода': 'прозрачная', 'Оптическая мощность': '80мВт', 'Монтаж': 'SMD', 'Размеры': '3,3x2,35x1,7мм', 'Ток диода LED': '100мА', '#Promotion': 'blackpool18', 'Поверхность': 'плоская', 'Рабочее напряжение': '1,5...1,8В', 'Обзор': '15°'}</t>
+          <t>www.tme.eu/ru/details/pr185-100r-a-p6/potentsiometry-odnooborotnye-ugolnye/telpod/pr185-100r-a-16p6/</t>
+        </is>
+      </c>
+      <c r="G14" s="3" t="inlineStr">
+        <is>
+          <t>{'Тип потенциометра': 'осевой', 'Сопротивление': '100Ом', 'Мощность': '200мВт', 'Погрешность': '±20%', 'Монтаж': 'под пайку', 'Диаметр оси': '6мм', 'Длина оси': '10мм', 'Характеристика': 'линейная', 'Размеры корпуса': 'Ø18x12мм', 'Длина резьбы': '6мм', 'Выводы': 'кольцевой', 'Материал дорожки': 'углеродистый', 'Характеристики потенциометров': 'моно', 'Вид оси': 'с насечкой', 'Угол поворота механический': '300°', 'Шаг выводов': '5,08мм', 'Длина оси L': '16мм', 'Рабочее напряжение макс.': '200В'}</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>www.tme.eu/Document/8779098747e6734be0de04691ff3714c/SFH4645.pdf</t>
+          <t>www.tme.eu/Document/62eccebcea8cd06ab95441901a40a7e0/PR185_16P6_3D.Pdf</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="2" t="inlineStr">
-        <is>
-          <t>SFH 4544</t>
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>WS2812D-F8</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>SFH4544</t>
+          <t>WS2812D-F8</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>ИК-передатчик; 5мм; 950нм; черная; 550мВт; 10°; THT; 100мА; 1,6÷1,9В</t>
+          <t>LED; 8мм; трехцветный; RGB; Характеристики: программируемый</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.000304</v>
+        <v>0.00078</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>static.tme.eu/products_pics/f/e/b/febde61e1b2a7ccd4dfe05ad78c6476d/492380.jpg</t>
+          <t>static.tme.eu/products_pics/f/3/3/f332dc60fb1b57c60944f1fca572f6ee/533326.jpg</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>www.tme.eu/ru/details/sfh4544/infrakrasnye-ledy/osram/sfh-4544/</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>{'Производитель': 'OSRAM', 'Тип диода': 'ИК-передатчик', 'Диаметр диода LED': '5мм', 'Длина волны λp': '950нм', 'Линза диода': 'черная', 'Оптическая мощность': '550мВт', 'Монтаж': 'THT', 'Ток диода LED': '100мА', '#Promotion': 'blackpool18', 'Поверхность': 'выпуклая', 'Рабочее напряжение': '1,6...1,9В', 'Обзор': '10°'}</t>
+          <t>www.tme.eu/ru/details/ws2812d-f8/svetodiody-tht-8mm/worldsemi/</t>
+        </is>
+      </c>
+      <c r="G15" s="3" t="inlineStr">
+        <is>
+          <t>{'Тип диода': 'LED', 'Диаметр диода LED': '8мм', 'Исполнение диода LED': 'трехцветный', 'Цвет диодa LED': 'RGB', 'Длина волны красного цвета λd': '620...630нм', 'Длина волны зеленого цвета λd': '515...530нм', 'Длина волны голубого цвета': '465...475нм', 'Монтаж': 'THT', 'Характеристики диодов LED': 'программируемый', '#Common #name - #search': 'управляемый', 'Рабочая температура': '-25...80°C', 'Кол-во цветов': '16,7M', 'Рабочее напряжение': '1,8..2,2/2,8..3,1/2,9..3,2В'}</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>www.tme.eu/Document/cfcc0d8a6669b62a22b9ffa1b7af2799/SFH4544.pdf</t>
+          <t>www.tme.eu/Document/ad9ae248bdf5411d99fdf954770e49ab/WS2812.txt</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="2" t="inlineStr">
-        <is>
-          <t>1-1393243-4</t>
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>IPP50R199CPXKSA1</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>RTE24110</t>
+          <t>IPP50R199CPXKSA1</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Реле: электромагнитное; DPDT; Uобмотки: 110ВDC; 8A/250ВAC; 8А; IP67</t>
+          <t>Транзистор: N-MOSFET; полевой; 500В; 17А; 139Вт; PG-TO220-3</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.014</v>
+        <v>0.00202</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>static.tme.eu/products_pics/c/1/c/c1cddf42b5c032463476cdf943894e36/636642.jpg</t>
+          <t>static.tme.eu/products_pics/8/1/5/81513517264a0a86329bb3b1e29800b3/59300.jpg</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>www.tme.eu/ru/details/rte24110/rele-elektromagn-miniatiurnye/te-connectivity/1-1393243-4/</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>{'Производитель': 'TE Connectivity', 'Тип реле': 'электромагнитное', 'Контакты': 'DPDT', 'Номинальное напряжение обмотки': '110В DC', 'Нагрузка контакта AC @R': '8A / 250В AC', 'Нагрузка контакта DC @R': '8A / 30В DC', 'Ток контактов макс.': '8А', 'Коммутируемое напряжение': 'макс. 400В AC', 'Исполнение реле': 'миниатюрное', 'Монтаж': 'PCB', 'Сопротивление обмотки макс.': '28,8кОм', 'Напряжение обмотки мин.': '77В DC', 'Время срабатывания': '8мс', 'Внешние размеры': '29x12,7x15,7мм', 'Время отпускания': '6мс', 'Мощность, потребляемая обмоткой': '420мВт', 'Класс защиты': 'IP67', 'Рабочая температура': '-40...85°C', 'Вес': '13г', 'Серия реле': 'RT2', 'Материал контакта': 'AgNi 90/10', '#Promotion': 'teconn_201912', 'Шаг выводов': '5мм', 'Высота': '15,7мм', 'Кол-во выводов': '8'}</t>
+          <t>www.tme.eu/ru/details/ipp50r199cpxksa1/tranzistory-s-kanalom-n-tht/infineon-technologies/</t>
+        </is>
+      </c>
+      <c r="G16" s="3" t="inlineStr">
+        <is>
+          <t>{'Тип транзистора': 'N-MOSFET', 'Технология': 'CoolMOS™', 'Полярность': 'полевой', 'Напряжение сток-исток': '500В', 'Ток стока': '17А', 'Рассеиваемая мощность': '139Вт', 'Корпус': 'PG-TO220-3', 'Напряжение затвор-исток': '±20В', 'Сопротивление в открытом состоянии': '0,199Ом', 'Монтаж': 'THT', 'Вид упаковки': 'туба', 'Вид канала': 'обогащенный'}</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>www.tme.eu/Document/20b30a5bf30586aa5a0833410fafc6af/IPP50R199CP-DTE.pdf</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="2" t="inlineStr">
-        <is>
-          <t>502578-0700</t>
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>IXTP60N20T</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>MX-502578-0700</t>
+          <t>IXTP60N20T</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Вилка; провод-плата; "мама"; CLIK-Mate; 1,5мм; PIN: 7; на провод</t>
+          <t>Транзистор: N-MOSFET; полевой; 200В; 60А; 500Вт; TO220-3; 118нс</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>0.00036</v>
+        <v>0.00205</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>static.tme.eu/products_pics/3/c/8/3c86273de4738928cb85ee55c6283721/424952.jpg</t>
+          <t>static.tme.eu/products_pics/5/1/e/51ec0da338efc7576395da0cb4cd6065/52963.jpg</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>www.tme.eu/ru/details/mx-502578-0700/razemy-signalnye-rastr-1-50mm/molex/502578-0700/</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>{'Производитель': 'MOLEX', '#Promotion': 'africa_anniversary', 'Разъем': 'вилка', 'Тип разъема': 'провод - плата', 'Вид разъемов': '"мама"', 'Серия разъема': 'CLIK-Mate', 'Шаг контактов': '1,5мм', 'Кол-во выводов': '7', 'Версия разъема': 'без контактов', 'Механический монтаж': 'на провод', 'Фиксация разъема': 'защелка', 'Рабочая температура': '-25...85°C', 'Конфигурация выводов разъема': '1x7', 'Дополнительная информация': 'больше товаров данной серии доступно на www.tme.eu', 'Alias': '5025780700', 'Engineering PN': '502578-0700'}</t>
+          <t>www.tme.eu/ru/details/ixtp60n20t/tranzistory-s-kanalom-n-tht/ixys/</t>
+        </is>
+      </c>
+      <c r="G17" s="3" t="inlineStr">
+        <is>
+          <t>{'Тип транзистора': 'N-MOSFET', 'Полярность': 'полевой', 'Напряжение сток-исток': '200В', 'Ток стока': '60А', 'Рассеиваемая мощность': '500Вт', 'Корпус': 'TO220-3', 'Сопротивление в открытом состоянии': '40мОм', 'Монтаж': 'THT', 'Заряд затвора': '73нC', 'Вид упаковки': 'туба', 'Вид канала': 'обогащенный', 'Характеристики полупроводниковых элементов': 'thrench gate power mosfet', 'Время готовности': '118нс'}</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>www.tme.eu/Document/6875713b1f30ff5ff87e2fe31c7f0235/5025780200_sd.pdf</t>
+          <t>www.tme.eu/Document/44812aae0db68a764b468669eda9603d/IXTA(P,Q)60N20T.pdf</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="2" t="inlineStr">
-        <is>
-          <t>503149-1000</t>
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>STP6NK60ZFP</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>MX-503149-1000</t>
+          <t>STP6NK60ZFP</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Вилка; провод-плата; "мама"; CLIK-Mate; 1,5мм; PIN: 10; на провод</t>
+          <t>Транзистор: N-MOSFET; полевой; 600В; 3,8А; 110Вт; TO220FP</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>0.00043</v>
+        <v>0.0017</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>static.tme.eu/products_pics/4/3/d/43d49000d63b29f4ddd39b9ae26883cf/424954.jpg</t>
+          <t>static.tme.eu/products_pics/d/b/6/db6e7e2b449fafc55decaa715c08590e/60491.jpg</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>www.tme.eu/ru/details/mx-503149-1000/razemy-signalnye-rastr-1-50mm/molex/503149-1000/</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>{'Производитель': 'MOLEX', '#Promotion': 'africa_anniversary', 'Разъем': 'вилка', 'Тип разъема': 'провод - плата', 'Вид разъемов': '"мама"', 'Серия разъема': 'CLIK-Mate', 'Шаг контактов': '1,5мм', 'Кол-во выводов': '10', 'Версия разъема': 'без контактов', 'Механический монтаж': 'на провод', 'Фиксация разъема': 'защелка', 'Рабочая температура': '-25...85°C', 'Конфигурация выводов разъема': '2x5', 'Дополнительная информация': 'больше товаров данной серии доступно на www.tme.eu', 'Alias': '5031491000', 'Engineering PN': '503149-1000'}</t>
+          <t>www.tme.eu/ru/details/stp6nk60zfp/tranzistory-s-kanalom-n-tht/stmicroelectronics/</t>
+        </is>
+      </c>
+      <c r="G18" s="3" t="inlineStr">
+        <is>
+          <t>{'Тип транзистора': 'N-MOSFET', 'Технология': 'SuperMesh™', 'Полярность': 'полевой', 'Напряжение сток-исток': '600В', 'Ток стока': '3,8А', 'Рассеиваемая мощность': '110Вт', 'Корпус': 'TO220FP', 'Напряжение затвор-исток': '±30В', 'Сопротивление в открытом состоянии': '1200мОм', 'Монтаж': 'THT', 'Вид упаковки': 'туба', 'Вид канала': 'обогащенный', 'Характеристики полупроводниковых элементов': 'ESD protected gate'}</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>www.tme.eu/Document/c33cc2020ff92d2ac74457cd277b7833/5031490800_sd.pdf</t>
+          <t>www.tme.eu/Document/3e2435781f07f0180cbe6444f8008c50/STP6NK60Z.pdf</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="2" t="inlineStr">
-        <is>
-          <t>171692-0106</t>
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>IRFP3006PBF</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>MX-171692-0106</t>
+          <t>IRFP3006PBF</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Вилка; провод-плата; "мама"; Mega-Fit; 5,7мм; PIN: 6; Конф: 2x3; 23А</t>
+          <t>Транзистор: N-MOSFET; полевой; 60В; 195А; 375Вт; TO247AC</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0.0035</v>
+        <v>0.0056</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>static.tme.eu/products_pics/0/2/5/025a1c5c7745ef6525f92e9062b39b6b/424939.jpg</t>
+          <t>static.tme.eu/products_pics/1/0/0/100fc9da60f9ae9d6488451decdc0742/52384.jpg</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>www.tme.eu/ru/details/mx-171692-0106/razemy-signalnye-rastr-5-70mm/molex/171692-0106/</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>{'Производитель': 'MOLEX', '#Promotion': 'africa_anniversary', 'Разъем': 'вилка', 'Тип разъема': 'провод - плата', 'Вид разъемов': '"мама"', 'Серия разъема': 'Mega-Fit', 'Шаг контактов': '5,7мм', 'Кол-во выводов': '6', 'Конфигурация выводов разъема': '2x3', 'Максимальный ток': '23А', 'Класс горючести': 'UL94V-0', 'Версия разъема': 'без контактов', 'Цвет': 'черный', 'Рабочая температура': '-40...105°C', 'Фиксация разъема': 'защелка', 'Механический монтаж': 'на провод', 'Пространственная ориентация': 'прямой', 'Дополнительная информация': 'больше товаров данной серии доступно на www.tme.eu', 'Alias': '1716920106', 'Engineering PN': '171692-0106'}</t>
+          <t>www.tme.eu/ru/details/irfp3006pbf/tranzistory-s-kanalom-n-tht/infineon-irf/</t>
+        </is>
+      </c>
+      <c r="G19" s="3" t="inlineStr">
+        <is>
+          <t>{'Тип транзистора': 'N-MOSFET', 'Технология': 'HEXFET®', 'Полярность': 'полевой', 'Напряжение сток-исток': '60В', 'Ток стока': '195А', 'Рассеиваемая мощность': '375Вт', 'Корпус': 'TO247AC', 'Напряжение затвор-исток': '±20В', 'Сопротивление в открытом состоянии': '2,1мОм', 'Монтаж': 'THT', 'Заряд затвора': '200нC', 'Вид упаковки': 'туба'}</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>www.tme.eu/Document/0498fc69ae72e4fa7ad609f215554d1e/Mega-Fit MOLEX.txt</t>
+          <t>www.tme.eu/Document/6c5acfff2f6970577e609dbbce91673c/IRFP3006PBF.pdf</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="2" t="inlineStr">
-        <is>
-          <t>226X65</t>
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>M22-FLED-RG</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>TFM-M4X65/DR226</t>
+          <t>M22-FLED-RG</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Дистанцирующая стойка с резьбой; Внутр.резьба: M4; 65мм; сталь</t>
+          <t>Элемент подсветки; 22мм; RMQ-Titan; -25÷70°C; Подсвет: LED; 24ВDC</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>0.0206</v>
+        <v>0.00387</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>static.tme.eu/products_pics/5/e/2/5e2cdfaad155e88dae96c532c2fabdd3/284846.jpg</t>
+          <t>static.tme.eu/products_pics/b/5/0/b50d39ae95205c9cdb74ac3175ce020b/546968.jpg</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>www.tme.eu/ru/details/tfm-m4x65_dr226/elementy-distantsionnye-metallicheskie/dremec/226x65/</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>{'Производитель': 'DREMEC', 'Тип распорнои стойки': 'дистанцирующая стойка с резьбой', 'Внутренняя резьба': 'M4', 'Расстояние между платами': '65мм', 'Внешняя резьба': 'M4', 'Форма стойки': 'шестигранная', 'Материал': 'сталь', 'Материал покрытия': 'цинк', 'Резьба + Длина - #wyszukiwanie': 'M4x65', '#Promotion': 'Spacers_forbot', 'Размер ключа': '7мм', 'Дополнительная информация': 'больше товаров данной серии доступно на www.tme.eu', 'Характеристики механических элементов': 'с внутренней и внешней резьбой'}</t>
+          <t>www.tme.eu/ru/details/m22-fled-rg/panelnye-aksessuary-standartnye/eaton-electric/</t>
+        </is>
+      </c>
+      <c r="G20" s="3" t="inlineStr">
+        <is>
+          <t>{'Тип аксессуаров для переключателей': 'элемент подсветки', 'Стандарт переключателя': '22мм', 'Серия производителя': 'RMQ-Titan', 'Рабочая температура': '-25...70°C', 'Подсветка': 'LED', 'Монтаж': 'фронтальный', 'Выводы': 'самозажимная клемма', 'Цвет диодa LED': 'красный/зеленый', 'Напряжение питания': '24В DC', 'Рабочий ток': '10...15мА', 'Характеристики переключателей': 'плоский', '#Common #name - #search': 'RMQ Flat Rear'}</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>www.tme.eu/Document/451757bfa0cf89650334b0f101e3f2bd/Dremec_13.pdf</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="30" r="21">
-      <c r="A21" s="2" t="inlineStr">
-        <is>
-          <t>LT1767EMS8E-5#PBF</t>
+          <t>www.tme.eu/Document/a0961acde83b0d03be17da458b112b27/M30C-YTB.txt</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>HER508</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>LT1767EMS8E5PBF</t>
+          <t>HER508</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>PMIC; преобразователь DC/DC; Uвх: 3÷25В; Uвых: 5В; MSOP8; buck</t>
+          <t>Диод: выпрямительный; THT; 1кВ; 5А; Упаковка: Ammo Pack; DO27; 100нс</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>2.4e-05</v>
+        <v>0.0011</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>static.tme.eu/products_pics/5/3/1/531d7915b61678c8109674b14bfbf850/285547.jpg</t>
+          <t>static.tme.eu/products_pics/c/a/9/ca9e994cf064bab176fe27dff82952ef/60318.jpg</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>www.tme.eu/ru/details/lt1767ems8e5pbf/reguliatory-napriazheniia-mikroskhemy-dc-dc/analog-devices-linear-technology/lt1767ems8e-5-pbf/</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>{'Производитель': 'Analog Devices (Linear Technology)', 'Тип микросхемы': 'PMIC', 'Вид микросхемы': 'преобразователь DC/DC', 'Входное напряжение': '3...25В', 'Выходное напряжение': '5В', 'Выходной ток': '1,5А', 'Частота': '1250кГц', 'Монтаж': 'SMD', 'Корпус': 'MSOP8', 'Топология': 'buck', 'Кол-во каналов': '1'}</t>
+          <t>www.tme.eu/ru/details/her508/universalnye-diody-tht/dc-components/</t>
+        </is>
+      </c>
+      <c r="G21" s="3" t="inlineStr">
+        <is>
+          <t>{'Тип диода': 'выпрямительный', 'Монтаж': 'THT', 'Обратное напряжение макс.': '1кВ', 'Прямой ток': '5А', 'Конструкция диода': 'одиночный диод', 'Характеристики полупроводниковых элементов': 'быстрое переключение', 'Вид упаковки': 'Ammo Pack', 'Корпус': 'DO27', 'Время готовности': '100нс', 'Импульсный ток': '150А', 'Падение напряжения макс.': '1,7В'}</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>www.tme.eu/Document/cfc3853de0a94ff4921db09d0d2742cc/lt1767.pdf</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="30" r="22">
-      <c r="A22" s="2" t="inlineStr">
-        <is>
-          <t>PF92251V1-1000U-G99</t>
+          <t>www.tme.eu/Document/b910c50b6b49fab4130a48499e482579/HER501-HER508-DTE.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>SP2111/S12 II 1N</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>PF92251V1-G99-A</t>
+          <t>SP2111/S12</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Вентилятор: DC; осевой; 12ВDC; 92x92x25мм; 126,75м3/ч; 45,5дБА</t>
+          <t>Вилка; "мама"; SP21; PIN: 12; IP68; 7÷12мм; пайка; на провод; 400В</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0.1092</v>
+        <v>0.0259</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>static.tme.eu/products_pics/5/d/e/5de68175009220d792b5fff4ea124a77/586569.jpg</t>
+          <t>static.tme.eu/products_pics/8/a/0/8a016c70def4dbb27e1b15243ea7225a/371417.jpg</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>www.tme.eu/ru/details/pf92251v1-g99-a/ventiliatory-dc-12v/sunon/pf92251v1-1000u-g99/</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>{'Производитель': 'SUNON', 'Тип вентилятора': 'DC', 'Вид вентилятора': 'осевой', 'Напряжение питания': '12В DC', 'Размер вентилятора': '92x92x25мм', 'Потребл. мощность': '4,44Вт', 'Номинальный ток': '0,37А', 'Воздушный поток': '126,75м&lt;sup&gt;3&lt;/sup&gt;/ч', 'Уровень шума': '45,5дБА', 'Вид подшипника': 'Vapo', 'Сигнальный вывод': 'Типа F', 'Скорость вращения': '4500об./мин.', 'Вес': '106г', 'Сопротивление изоляции мин.': '10МОм', 'Материал крыльчатки': 'термопласт', 'Материал корпуса': 'термопласт', 'Класс изоляции': 'A', 'Выводы': '3 провода', 'Рабочая температура': '-10...70°C', 'Длина провода': '305мм', 'Статическое давление': '8,89мм H&lt;sub&gt;2&lt;/sub&gt;O', 'Мотор вентилятора': 'бесколлекторный, DC', 'Класс горючести': 'UL94V-0', 'Дополнительные функции': 'автоперезапуск', 'Рабочее напряжение': '6...13,8В', 'Размер провода': '24AWG'}</t>
+          <t>www.tme.eu/ru/details/sp2111_s12/razemy-weipu/weipu/sp2111-s12-ii-1n/</t>
+        </is>
+      </c>
+      <c r="G22" s="3" t="inlineStr">
+        <is>
+          <t>{'Тип разъема': 'круглый', 'Разъем': 'вилка', 'Вид разъемов': '"мама"', 'Серия разъема': 'SP21', 'Кол-во выводов': '12', 'Класс защиты': 'IP68', 'Внешний диаметр провода': '7...12мм', 'Электрический монтаж': 'пайка', 'Механический монтаж': 'на провод', 'Номинальное напряжение': '400В', 'Дополнительная информация': 'больше товаров данной серии доступно на www.tme.eu', 'Фиксация разъема': 'резьбовая', 'Сечение провода 1': '0,75мм&lt;sup&gt;2&lt;/sup&gt;', 'Номинальный ток 1': '5А', 'Рабочая температура': '-25...85°C'}</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>www.tme.eu/Document/669ceba5964765359ee39d8b0b038d57/PF92251V1-1000U-G99 D09034460G-00.pdf</t>
+          <t>www.tme.eu/Document/695668426cf2efe008d7e70b952aa241/SP21.pdf</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="2" t="inlineStr">
-        <is>
-          <t>L-934SRD-E</t>
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>SP2111/P12 II 1N</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>SP2111/P12</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Артикула нет на TME</t>
+          <t>Вилка; "папа"; SP21; PIN: 12; IP68; 7÷12мм; пайка; на провод; 400В</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>0.0217</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>static.tme.eu/products_pics/c/8/9/c8962e0e9f0cd9242036587606afbf14/416835.jpg</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>www.tme.eu/ru/details/sp2111_p12/razemy-weipu/weipu/sp2111-p12-ii-1n/</t>
+        </is>
+      </c>
+      <c r="G23" s="3" t="inlineStr">
+        <is>
+          <t>{'Тип разъема': 'круглый', 'Разъем': 'вилка', 'Вид разъемов': '"папа"', 'Серия разъема': 'SP21', 'Кол-во выводов': '12', 'Класс защиты': 'IP68', 'Внешний диаметр провода': '7...12мм', 'Электрический монтаж': 'пайка', 'Механический монтаж': 'на провод', 'Номинальное напряжение': '400В', 'Дополнительная информация': 'больше товаров данной серии доступно на www.tme.eu', 'Фиксация разъема': 'резьбовая', 'Сечение провода 1': '0,75мм&lt;sup&gt;2&lt;/sup&gt;', 'Номинальный ток 1': '5А', 'Рабочая температура': '-25...85°C'}</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>www.tme.eu/Document/695668426cf2efe008d7e70b952aa241/SP21.pdf</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="2" t="inlineStr">
-        <is>
-          <t>ULN2004A</t>
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>KQ2L06-M5A</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>ULN2004A</t>
+          <t>KQ2L06-M5A</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Driver; darlington,транзисторная матрица; 0,5А; 50В; Каналы: 7</t>
+          <t>Быстроразъемное соединение; с резьбой,угловой 90°; M5; внешняя</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>0.00101</v>
+        <v>0.00329</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>static.tme.eu/products_pics/7/f/8/7f875655d065e0178d8b518f0dda4bec/201862.jpg</t>
+          <t>static.tme.eu/products_pics/4/0/4/4040bae49fed6597a4b6588ac4c5ea09/381784.jpg</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>www.tme.eu/ru/details/uln2004a/draivery-mikroskhemy/stmicroelectronics/</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>{'Производитель': 'STMicroelectronics', 'Тип микросхемы': 'driver', 'Вид микросхемы': 'транзисторная матрица', 'Выходной ток': '0,5А', 'Выходное напряжение': '50В', 'Кол-во каналов': '7', 'Монтаж': 'THT', 'Рабочая температура': '-40...85°C', 'Входное напряжение': '30В', 'Корпус': 'DIP16'}</t>
+          <t>www.tme.eu/ru/details/kq2l06-m5a/razemy-i-provoda/smc/</t>
+        </is>
+      </c>
+      <c r="G24" s="3" t="inlineStr">
+        <is>
+          <t>{'Тип аксессуаров для пневматики': 'быстроразъемное соединение', 'Версия соединителя': 'угловой 90°', 'Резьба': 'M5', 'Вид резьбы': 'внешняя', 'Внешний диаметр провода': '6мм', 'Рабочее давление': '-1...10бар', 'Рабочая температура': '-5...60°C', 'Материал корпуса': 'полипропилен', 'Характеристики элементов пневматики': 'поворотный на 360°'}</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>www.tme.eu/Document/59932c7719cf25b6baad20a181aaae88/ULN200x.pdf</t>
+          <t>www.tme.eu/Document/44caf5003dc345c4787b2e3bea23bf51/KQ2-SERIES.pdf</t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="2" t="inlineStr">
-        <is>
-          <t>39-30-0060</t>
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>PMEG4005AEV.115</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>MX-39-30-0060</t>
+          <t>PMEG4005AEV.115</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Гнездо; провод-плата; "папа"; Mini-Fit Jr; 4,2мм; PIN: 6; THT; 13А</t>
+          <t>Диод: выпрямительный Шоттки; SMD; 40В; 0,5А; Ufmax: 0,47В; SOT666</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>0.0023</v>
+        <v>2.9e-05</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>static.tme.eu/products_pics/1/8/5/185e65bc40581880c4f2c82958de8cfe/746.jpg</t>
+          <t>static.tme.eu/products_pics/e/0/6/e06ceaa63cab65ded13f2b20b1fdd688/418864.jpg</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>www.tme.eu/ru/details/mx-39-30-0060/razemy-signalnye-rastr-4-20mm/molex/39-30-0060/</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>{'Производитель': 'MOLEX', '#Promotion': 'africa_anniversary', 'Разъем': 'гнездо', 'Тип разъема': 'провод - плата', 'Вид разъемов': '"папа"', 'Серия разъема': 'Mini-Fit Jr.', 'Шаг контактов': '4,2мм', 'Кол-во выводов': '6', 'Электрический монтаж': 'THT', 'Максимальный ток': '13А', 'Покрытие контакта': 'луженые', 'Класс горючести': 'UL94V-0', 'Фиксация разъема': 'защелка', 'Конфигурация выводов разъема': '2x3', 'Дополнительная информация': 'больше товаров данной серии доступно на www.tme.eu', 'Alias': '39300060', 'Engineering PN': '5569-06A2-210', 'Пространственная ориентация': 'угловой 90°'}</t>
+          <t>www.tme.eu/ru/details/pmeg4005aev.115/diody-shotki-smd/nexperia/</t>
+        </is>
+      </c>
+      <c r="G25" s="3" t="inlineStr">
+        <is>
+          <t>{'Тип диода': 'выпрямительный Шоттки', 'Монтаж': 'SMD', 'Обратное напряжение макс.': '40В', 'Прямой ток': '0,5А', 'Конструкция диода': 'одиночный диод', 'Падение напряжения макс.': '0,47В', 'Корпус': 'SOT666', 'Вид упаковки': 'лента', 'Импульсный ток': '3,5А'}</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>www.tme.eu/Document/dc1bd2993ed47b1262da95547174c200/MX-39-30-0060.pdf</t>
+          <t>www.tme.eu/Document/1f193c68b39b55a6895795f54aa64c8b/PMEG4005AEV-DTE.pdf</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="2" t="inlineStr">
-        <is>
-          <t>42816-0412</t>
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>RDA-S4-W2-B</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>MX-42816-0412</t>
+          <t>RDA-S4-W2-B</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Вилка; провод-плата; "мама"; Серия: Mini-Fit Sr; 10мм; PIN: 4; 600В</t>
+          <t>Адаптер; гнездо "банан" 4мм,вилочный наконечник; 60ВDC; 36А</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>0.01074</v>
+        <v>0.00296</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>static.tme.eu/products_pics/9/c/6/9c6840ea15823045d1db990f774bd7f3/366649.jpg</t>
+          <t>static.tme.eu/products_pics/5/1/2/5129e8bee14a5556b25023ddb90411c4/40195.jpg</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>www.tme.eu/ru/details/mx-42816-0412/razemy-signalnye-rastr-10mm/molex/42816-0412/</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>{'Производитель': 'MOLEX', '#Promotion': 'africa_anniversary', 'Разъем': 'вилка', 'Тип разъема': 'провод - плата', 'Вид разъемов': '"мама"', 'Серия разъема': 'Mini-Fit Sr.', 'Шаг контактов': '10мм', 'Кол-во выводов': '4', 'Alias': '428160412', 'Engineering PN': '42816-0412', 'Номинальное напряжение': '600В', 'Механический монтаж': 'на провод', 'Рабочая температура': '-40...105°C', 'Версия разъема': 'без контактов'}</t>
-        </is>
-      </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>www.tme.eu/Document/1f6b35bb6f23de72d8f577f3719e1057/mx42816.pdf</t>
+          <t>www.tme.eu/ru/details/rda-s4-w2-b/shtepselnye-vilki/</t>
+        </is>
+      </c>
+      <c r="G26" s="3" t="inlineStr">
+        <is>
+          <t>{'Тип измерительных аксессуаров': 'адаптер', 'Конструкция кабеля / переходника': 'гнездо "банан" 4мм', 'Номинальный ток': '36А', 'Цвет': 'черный', 'Длина': '43мм', 'Покрытие контакта': 'никелированные', 'Материал контакта': 'латунь', 'Материал изолятора': 'полиамид', 'Номинальное напряжение': '60В DC'}</t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="2" t="inlineStr">
-        <is>
-          <t>T910W-20K</t>
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>RDA-S4-W2-B</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>T910W-20K</t>
+          <t>RDA-S4-W2-B</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Потенциометр: монтажный; многооборотный; 20кОм; 500мВт; THT; ±10%</t>
+          <t>Адаптер; гнездо "банан" 4мм,вилочный наконечник; 60ВDC; 36А</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>0.00076</v>
+        <v>0.00296</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>static.tme.eu/products_pics/8/7/9/879f983ff716a8c18d22787ca4396591/346620.jpg</t>
+          <t>static.tme.eu/products_pics/5/1/2/5129e8bee14a5556b25023ddb90411c4/40195.jpg</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>www.tme.eu/ru/details/t910w-20k/potentsiometry-tht-mnogooborotnye-3-8-dm/sr-passives/</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>{'Производитель': 'SR PASSIVES', 'Тип потенциометра': 'монтажный', 'Вид потенциометра': 'многооборотный', 'Сопротивление': '20кОм', 'Мощность': '500мВт', 'Монтаж': 'THT', 'Погрешность': '±10%', 'Характеристика': 'линейная', 'Материал дорожки': 'металлокерамический', 'Рабочая температура': '-55...125°C', 'Стандарт потенциометра': '3/8"', 'Температурный коэффициент': '100ppm/°C', 'Размеры корпуса': '10x9,5x4,8мм', 'Шаг выводов': '2,5мм', 'Количество оборотов механич.': '28', 'Аналоги других производителей': 'T93YA', 'Регулировка': 'вертикальная', 'Ресурс': '200циклов'}</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>www.tme.eu/Document/46e9ecf29426285f0ed14cb1dbb4a9ca/SR_Passives-T910.pdf</t>
+          <t>www.tme.eu/ru/details/rda-s4-w2-b/shtepselnye-vilki/</t>
+        </is>
+      </c>
+      <c r="G27" s="3" t="inlineStr">
+        <is>
+          <t>{'Тип измерительных аксессуаров': 'адаптер', 'Конструкция кабеля / переходника': 'гнездо "банан" 4мм', 'Номинальный ток': '36А', 'Цвет': 'черный', 'Длина': '43мм', 'Покрытие контакта': 'никелированные', 'Материал контакта': 'латунь', 'Материал изолятора': 'полиамид', 'Номинальное напряжение': '60В DC'}</t>
         </is>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="2" t="inlineStr">
-        <is>
-          <t>TR-20-SM</t>
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>ILM12F-DOE-635-7-247-F</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>TR-20-SM</t>
+          <t>ILM12F-C-635-7-247</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Губцевый; для резки,миниатюрные; Дл.инструмента: 140мм</t>
+          <t>Модуль: лазерный; 7мВт; красный; крест; 635нм; 4,5÷30ВDC; IP54</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>0.0503</v>
+        <v>0.0302</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>static.tme.eu/products_pics/a/8/4/a84fb90a10c7b1595db87c69d4e98dbb/281726.jpg</t>
+          <t>static.tme.eu/products_pics/7/e/f/7ef35f30eda27eac8adf78fba3ab6fd0/435944.jpg</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>www.tme.eu/ru/details/tr-20-sm/kleshchi-kusachki-dlia-rezki/piergiacomi/</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>{'Производитель': 'PIERGIACOMI', 'Тип инструмента': 'губцевый', 'Вид губцевый': 'миниатюрные', 'Характеристики щипцов/ножей': 'ручки с двухкомпонентными накладками эргономичной формы с противоскользящим верхним слоем', 'Диапазон резки': 'медная проволока диаметром до 0,8мм', 'Длина инструмента': '140мм', '#Promotion': 'electricians_day_201906'}</t>
+          <t>www.tme.eu/ru/details/ilm12f-c-635-7-247/moduli-lazernye/laser-components/ilm12f-doe-635-7-247-f/</t>
+        </is>
+      </c>
+      <c r="G28" s="3" t="inlineStr">
+        <is>
+          <t>{'Тип модуля': 'лазерный', 'Мощность': '7мВт', 'Цвет': 'красный', 'Оптическая головка': 'крест', 'Длина волны λd': '635нм', 'Напряжение питания': '4,5...30В DC', 'Характеристики оптоэлектронных модулей': 'возможна коллимация пучка', 'Применение': 'системы сигнализации', 'Внешние размеры': 'Ø12x68мм', 'Серия производителя': 'FLEXPOINT®', 'Серия': 'ILM12F', 'Электрическое подключение': 'разъем М12 4pin', 'Класс защиты': 'IP54'}</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>www.tme.eu/Document/3283c0440d53f053bb6c880de2756158/TR-20-SM.pdf</t>
+          <t>www.tme.eu/Document/6fbb8f9664555bf33195763088a09479/ILM12F.pdf</t>
         </is>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="2" t="inlineStr">
-        <is>
-          <t>SFH620A-3</t>
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>PIC16F1933-I/SO</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>SFH620A-3</t>
+          <t>PIC16F1933-I/SO</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Оптрон; THT; Каналы: 1; Вых: транзисторный; Uизол: 5,3кВ; Uce: 70В</t>
+          <t>Микроконтроллер PIC; Память: 7кБ; SRAM: 256Б; EEPROM: 256Б; SMD</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>0.00024</v>
+        <v>0.00079</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>static.tme.eu/products_pics/d/2/5/d25df74059f2c953ae3361deb72a98d6/285339.jpg</t>
+          <t>static.tme.eu/products_pics/8/1/0/81051b9be20cf4a4329cccddb66e4d6e/285347.jpg</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>www.tme.eu/ru/details/sfh620a-3/optrony-analogovyi-vykhod/vishay/</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>{'Производитель': 'VISHAY', 'Тип полупроводникового элемента': 'оптрон', 'Монтаж': 'THT', 'Кол-во каналов': '1', 'Вид выхода': 'транзисторный', 'Напряжение изоляции': '5,3кВ', 'CTR@If': '4.5%@1mA', 'Напряжение коллектор-эмиттер': '70В', 'Корпус': 'DIP4', 'Время включения': '3мкс', 'Время выключения': '2,3мкс'}</t>
+          <t>www.tme.eu/ru/details/pic16f1933-i_so/lineika-pic-8-bit/microchip-technology/</t>
+        </is>
+      </c>
+      <c r="G29" s="3" t="inlineStr">
+        <is>
+          <t>{'Тип микросхемы': 'микроконтроллер PIC', 'Память программы': '7кБ', 'Объем памяти SRAM': '256Б', 'Объем памяти EEPROM': '256Б', 'Интерфейс': 'MSSP (SPI / I2C)', 'Монтаж': 'SMD', 'Корпус': 'SO28', 'Кол-во входов/выходов': '25', 'Кол-во таймеров 8бит': '4', 'Кол-во таймеров 16бит': '1', 'Вид архитектуры': 'Harvard  8бит', 'Встроенный генератор': '32МГц', 'Семейство': 'PIC16', 'Рабочее напряжение': '1,8...5,5В'}</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>www.tme.eu/Document/dee9b38586ed8839c054de1e912b26dd/SFH6206-1.pdf</t>
-        </is>
-      </c>
-    </row>
+          <t>www.tme.eu/Document/4d0c5c72ca8112c45547387f903c5f34/PIC16F1933-I_ML.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>LTE-4206</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>LTE-4206</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>ИК-передатчик; 3мм; 940нм; прозрачная; 1,383÷7,67мВт; 20°; THT</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>0.00013</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>static.tme.eu/products_pics/3/3/1/331a414da4e5c4e20cf7de4b481b5806/438588.jpg</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>www.tme.eu/ru/details/lte-4206/infrakrasnye-ledy/liteon/</t>
+        </is>
+      </c>
+      <c r="G30" s="3" t="inlineStr">
+        <is>
+          <t>{'Тип диода': 'ИК-передатчик', 'Диаметр диода LED': '3мм', 'Длина волны λp': '940нм', 'Линза диода': 'прозрачная', 'Оптическая мощность': '1,383...7,67мВт', 'Монтаж': 'THT', 'Ток диода LED': '20мА', 'Рабочее напряжение': '1,2...1,6В', 'Обзор': '20°'}</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>www.tme.eu/Document/3a5cb70dcd89a87a28d68e3f0594b7ea/LTE-4206.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>RT-125C</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>RT-125C</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Блок питания: импульсный; модульный; 132,5Вт; 5ВDC; 199x98x38мм</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>0.6765</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>static.tme.eu/products_pics/2/1/0/2104fc19b06369c0cb2d4fde08c9f087/338613.jpg</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>www.tme.eu/ru/details/rt-125c/bloki-pitaniia-dlia-vstraivaniia/mean-well/</t>
+        </is>
+      </c>
+      <c r="G31" s="3" t="inlineStr">
+        <is>
+          <t>{'Тип блока питания': 'импульсный', 'Вид блока питания': 'модульный', 'Мощность': '132,5Вт', 'Внешние размеры': '199x98x38мм', 'Выходное напряжение 2': '15В DC', 'Выходное напряжение 3': '-15В DC', 'Выходной ток': '10 (2...15)А', 'Ток на выходе 2': '4,5 (0,5...6)А', 'Ток на выходе 3': '1 (0,1...1)А', 'Характеристики блоков питания/преобразователей': 'блок питания имеет несколько выходов, для корректной работы необходимо обеспечить нагрузку всех выходов в соответствующем диапазоне', 'Вес': '700г', 'Рабочая температура': '-25...70°C', 'Количество выходов': '3', 'Электрическое подключение': 'клеммная колодка', 'Монтаж': 'открытое исполнение', 'Защита': 'от увеличения напряжения', 'Напряжение питания': '248...373В DC', 'КПД': '81%', 'Серия': 'RT-125', 'Вид корпуса': '902-RT', 'Сопутствующие товары': 'DRP-03', 'Выходное напряжение': '5В DC'}</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>www.tme.eu/Document/ee6f0e6a23c81f0c481af689425f21b2/INB-MN-ENCLOSED-RU.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>LNS-1</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>LNS-1</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Набор заклепок</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>0.0067</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>static.tme.eu/products_pics/5/b/c/5bc907842357e38bba9ca847cdd4520e/544928.jpg</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>www.tme.eu/ru/details/lns-1/zaklepki/ht-hi-tech-polymers-oy/</t>
+        </is>
+      </c>
+      <c r="G32" s="3" t="inlineStr">
+        <is>
+          <t>{'Тип крепежного элемента': 'набор заклепок', 'Назначение': 'HTPC-16'}</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>www.tme.eu/Document/12c90dcac9056a2eb26687b38a6ec019/LNS-1.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Z24A</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Z24AN-ABS</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Корпус: универсальный; Х: 47мм; Y: 66мм; Z: 25мм; ABS</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>0.031</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>static.tme.eu/products_pics/c/d/d/cddd73d949b130e20718c43f58495ae6/576301.jpg</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>www.tme.eu/ru/details/z24an-abs/korpusa-universalnye/kradex/z24an-abs/</t>
+        </is>
+      </c>
+      <c r="G33" s="3" t="inlineStr">
+        <is>
+          <t>{'Тип корпуса': 'универсальный', 'Размер Х': '47мм', 'Размер Y': '66мм', 'Размер Z': '25мм', 'Материал корпуса': 'ABS', 'Цвет корпуса': 'голубой полупрозрачный'}</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>www.tme.eu/Document/82a304249f020c892dcfcd20554d6c99/Z24A.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>MF40201V2-1000U-A99</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>MF40201V2-A99-A</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Вентилятор: DC; осевой; 12ВDC; 40x40x20мм; 13,01м3/ч; 21дБА; Vapo</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>0.0285</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>static.tme.eu/products_pics/f/a/1/fa1a93887b02011e97d3a4ca780bf5be/582036.jpg</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>www.tme.eu/ru/details/mf40201v2-a99-a/ventiliatory-dc-12v/sunon/mf40201v2-1000u-a99/</t>
+        </is>
+      </c>
+      <c r="G34" s="3" t="inlineStr">
+        <is>
+          <t>{'Тип вентилятора': 'DC', 'Вид вентилятора': 'осевой', 'Напряжение питания': '12В DC', 'Размер вентилятора': '40x40x20мм', 'Потребл. мощность': '0,54Вт', 'Номинальный ток': '0,045А', 'Воздушный поток': '13,01м&lt;sup&gt;3&lt;/sup&gt;/ч', 'Уровень шума': '21дБА', 'Вид подшипника': 'Vapo', 'Скорость вращения': '6000об./мин.', 'Вес': '29г', 'Сопротивление изоляции мин.': '10МОм', 'Материал крыльчатки': 'термопласт', 'Материал корпуса': 'термопласт', 'Класс изоляции': 'A', 'Выводы': '2 провода', 'Рабочая температура': '-10...70°C', 'Длина провода': '305мм', 'Статическое давление': '4,32мм H&lt;sub&gt;2&lt;/sub&gt;O', 'Мотор вентилятора': 'бесколлекторный, DC', 'Класс горючести': 'UL94V-0', 'Дополнительные функции': 'автоперезапуск', 'Рабочее напряжение': '4,5...13,8В', 'Размер провода': '26AWG'}</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>www.tme.eu/Document/bcbab32aa9d675b07c94b6c48fd7ff55/MF40201V2-1000U-A99 D04111390G-00.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>LPF-90-42</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>LPF-90-42</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Блок питания: импульсный; LED; 90,3Вт; 42ВDC; 2,15А; 90÷305ВAC</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>0.6646</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>static.tme.eu/products_pics/1/c/4/1c40df3c355ea8b41869501850048eca/150631.jpg</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>www.tme.eu/ru/details/lpf-90-42/bloki-pitaniia-dlia-led/mean-well/</t>
+        </is>
+      </c>
+      <c r="G35" s="3" t="inlineStr">
+        <is>
+          <t>{'Тип блока питания': 'импульсный', 'Применение': 'LED', 'Вид блока питания': 'CV+CC', 'Мощность': '90,3Вт', 'Выходное напряжение': '42В DC', 'Выходной ток': '2,15А', 'Напряжение питания': '127...431В DC', 'Класс защиты': 'IP67', 'Внешние размеры': '61x161x36мм', 'Характеристики блоков питания/преобразователей': 'номинальные параметры при полной нагрузке', 'Защита': 'от увеличения напряжения', 'Вес': '700г', 'Рабочая температура': '-40...70°C', 'Электрическое подключение': 'провода 300мм', 'Количество выходов': '1', 'Дополнительные функции': 'активное PFC', 'Серия': 'LPF-90', 'КПД': '91%'}</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>www.tme.eu/Document/8f6b9eb035fb2946c20da9fe547dba90/INB-MN-LED-RU.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>IXFH26N60P</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>IXFH26N60P</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Транзистор: N-MOSFET; PolarHV™; полевой; 600В; 26А; 460Вт; TO247-3</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>0.00623</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>static.tme.eu/products_pics/d/8/b/d8bbc276e322c3e8c22886df1d4e31d5/16338.jpg</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>www.tme.eu/ru/details/ixfh26n60p/tranzistory-s-kanalom-n-tht/ixys/</t>
+        </is>
+      </c>
+      <c r="G36" s="3" t="inlineStr">
+        <is>
+          <t>{'Тип транзистора': 'N-MOSFET', 'Технология': 'PolarHV™', 'Полярность': 'полевой', 'Напряжение сток-исток': '600В', 'Ток стока': '26А', 'Рассеиваемая мощность': '460Вт', 'Корпус': 'TO247-3', 'Напряжение затвор-исток': '±30В', 'Сопротивление в открытом состоянии': '270мОм', 'Монтаж': 'THT', 'Заряд затвора': '72нC', 'Вид упаковки': 'туба', 'Вид канала': 'обогащенный', 'Время готовности': '200нс'}</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>www.tme.eu/Document/2af6871ed996921978a504d521ce54d3/IXFH26N60P.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>SS49E</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>SS49E</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Датчик: Холла; Диапазон: ±1000Гс; Uпит: 3÷6,5ВDC; 6мА</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>0.000104</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>static.tme.eu/products_pics/0/c/e/0ceb1f77d747ee63f0513d0a22097555/213063.jpg</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>www.tme.eu/ru/details/ss49e/datchiki-kholla/honeywell/</t>
+        </is>
+      </c>
+      <c r="G37" s="3" t="inlineStr">
+        <is>
+          <t>{'Тип датчика': 'Холла', 'Порог срабатывания': '±1000Гс', 'Напряжение питания': '3...6,5В DC', 'Коммутируемый ток': '6мА', 'Рабочая температура': '-40...100°C', 'Конфигурация выхода': 'линейный'}</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>www.tme.eu/Document/30447c50e7b2c9690d917bb3f82c99fe/ss49e-ss59et.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>MEGAVAL 175A</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>MEGAVAL-175A</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Предохранитель: плавкая вставка; 175А; 32В; автомобильный; 68,6мм</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>0.0182</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>static.tme.eu/products_pics/d/c/e/dce26399da05949750cfde69677994b1/512973.jpg</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>www.tme.eu/ru/details/megaval-175a/drugie-avtomobilnye-predokhraniteli/mta/megaval-175a/</t>
+        </is>
+      </c>
+      <c r="G38" s="3" t="inlineStr">
+        <is>
+          <t>{'Тип предохранителя': 'плавкая вставка', 'Номинальный ток': '175А', 'Номинальное напряжение': '32В', 'Вид предохранителя': 'автомобильный', 'Размер предохранителя': '68,6мм', 'Цвет': 'белый', '#Alternative #product': '0701175'}</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>www.tme.eu/Document/847cfb57c4200095ba005d9b3e4046d5/MTA_Product_catalogue_2018_s.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>MIDIVAL 30A</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>MIDIVAL-30A</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Предохранитель: плавкая вставка; 30А; 32В; автомобильный; 40мм</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>0.00618</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>static.tme.eu/products_pics/a/1/f/a1f4e00e9208bf770f5d6469b05c0a93/31963.jpg</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>www.tme.eu/ru/details/midival-30a/drugie-avtomobilnye-predokhraniteli/mta/midival-30a/</t>
+        </is>
+      </c>
+      <c r="G39" s="3" t="inlineStr">
+        <is>
+          <t>{'Тип предохранителя': 'плавкая вставка', 'Номинальный ток': '30А', 'Номинальное напряжение': '32В', 'Вид предохранителя': 'автомобильный', 'Размер предохранителя': '40мм', 'Цвет': 'оранжевый', 'Серия производителя': 'MIDIVAL', 'Рабочая температура': '-40...125°C', '#Alternative #product': '0702030', 'Монтаж': 'винт М5'}</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>www.tme.eu/Document/847cfb57c4200095ba005d9b3e4046d5/MTA_Product_catalogue_2018_s.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>RHS25RE</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>RHS25RE</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Потенциометр: осевой; однооборотный; 25Ом; 25Вт; 6,35мм; L: 22,23мм</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>0.0914</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>static.tme.eu/products_pics/d/7/2/d7275bd2e8b0e3a9de56374913ccc0f3/232722.jpg</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>www.tme.eu/ru/details/rhs25re/potentsiometry-odnooborotnye-provolochnye/ohmite/</t>
+        </is>
+      </c>
+      <c r="G40" s="3" t="inlineStr">
+        <is>
+          <t>{'Тип потенциометра': 'осевой', 'Вид потенциометра': 'однооборотный', 'Сопротивление': '25Ом', 'Мощность': '25Вт', 'Диаметр оси': '6,35мм', 'Характеристика': 'линейная', 'Размеры корпуса': 'Ø39,6x34,9мм', 'Длина резьбы': '9,53мм', 'Длина оси': '12,7мм', 'Вид оси': 'D профиль', 'Материал дорожки': 'проволочный', 'Монтажная резьба': '3/8"x32UNEF', 'Длина оси L': '22,23мм'}</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>www.tme.eu/Document/328be2551b00c340473695a498623641/controls_rheostats.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>MAX660CSA+</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>MAX660CSA+</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>PMIC; преобразователь DC/DC; Uвх: 1,5÷5,5В; Uвых: -5,5÷11В; SO8</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>9.000000000000001e-05</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>static.tme.eu/products_pics/4/8/a/48a33ccfb5a851d5982dcdda0776f7ac/285338.jpg</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>www.tme.eu/ru/details/max660csa+/reguliatory-napriazheniia-mikroskhemy-dc-dc/maxim-integrated/</t>
+        </is>
+      </c>
+      <c r="G41" s="3" t="inlineStr">
+        <is>
+          <t>{'Тип микросхемы': 'PMIC', 'Вид микросхемы': 'преобразователь DC/DC', 'Входное напряжение': '1,5...5,5В', 'Выходное напряжение': '-5,5...11В', 'Выходной ток': '0,1А', 'Частота': '80кГц', 'Мощность': '727мВт', 'Монтаж': 'SMD', 'Корпус': 'SO8', 'Топология': 'зарядовый насос', 'Кол-во каналов': '1'}</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>www.tme.eu/Document/c63992d00f9f1caeaa27e03fa0288e51/MAX660CPA+.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>MAX887HESA+</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>MAX887HESA+</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>PMIC; преобразователь DC/DC; Uвх: 3,5÷11В; Uвых: 1,25÷10В; SO8</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>8.000000000000001e-05</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>static.tme.eu/products_pics/4/8/a/48a33ccfb5a851d5982dcdda0776f7ac/285338.jpg</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>www.tme.eu/ru/details/max887hesa+/reguliatory-napriazheniia-mikroskhemy-dc-dc/maxim-integrated/</t>
+        </is>
+      </c>
+      <c r="G42" s="3" t="inlineStr">
+        <is>
+          <t>{'Тип микросхемы': 'PMIC', 'Вид микросхемы': 'преобразователь DC/DC', 'Входное напряжение': '3,5...11В', 'Выходное напряжение': '1,25...10В', 'Выходной ток': '0,6А', 'Частота': '300кГц', 'Мощность': '471мВт', 'Монтаж': 'SMD', 'Корпус': 'SO8', 'Топология': 'buck', 'Кол-во каналов': '1'}</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>www.tme.eu/Document/9259e352f7af53de65a77e93b3a57dd6/MAX887HESA+.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>PN2222ATA</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>PN2222ATA</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Транзистор: NPN; биполярный; 40В; 1А; 625мВт; TO92</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>0.00027</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>static.tme.eu/products_pics/b/1/4/b14f59eced0d57fc3010e7682ca65167/403830.jpg</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>www.tme.eu/ru/details/pn2222ata/tranzistory-npn-tht/on-semiconductor-fairchild/</t>
+        </is>
+      </c>
+      <c r="G43" s="3" t="inlineStr">
+        <is>
+          <t>{'Тип транзистора': 'NPN', 'Полярность': 'биполярный', 'Напряжение коллектор-эмиттер': '40В', 'Ток коллектора': '1А', 'Рассеиваемая мощность': '625мВт', 'Корпус': 'TO92', 'Монтаж': 'THT', 'Вид упаковки': 'Ammo Pack'}</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>www.tme.eu/Document/6fc4d4bda1f7e53502c9939019a00d3f/PN2222ABU.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>PMS 0.64</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>PMS0.64</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Изм.аксесс: измерительный набор; черный и красный</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>0.0455</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>static.tme.eu/products_pics/6/8/e/68e430d252100da0095ea4e60cc8b3a0/558089.jpg</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>www.tme.eu/ru/details/pms0.64/nabory-izmer-provodov-s-aksessuarami/hirschmann-t-m/pms-0-64/</t>
+        </is>
+      </c>
+      <c r="G44" s="3" t="inlineStr">
+        <is>
+          <t>{'Тип измерительных аксессуаров': 'измерительный набор', 'Цвет': 'черный и красный', 'Состав набора': 'зажим "крокодил" AGF1'}</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>www.tme.eu/Document/ba8ec780a8f7d34bd6e4df668539bb31/PMS 0,64_932959001.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>HRP-300-36</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>HRP-300-36</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Блок питания: импульсный; модульный; 324Вт; 36ВDC; 199x105x41мм</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>0.9294</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>static.tme.eu/products_pics/e/5/a/e5aa7b418aaaa5df9965fd365caaf850/413931.jpg</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>www.tme.eu/ru/details/hrp-300-36/bloki-pitaniia-dlia-vstraivaniia/mean-well/</t>
+        </is>
+      </c>
+      <c r="G45" s="3" t="inlineStr">
+        <is>
+          <t>{'Тип блока питания': 'импульсный', 'Вид блока питания': 'модульный', 'Мощность': '324Вт', 'Внешние размеры': '199x105x41мм', 'Выходной ток': '9А', 'Характеристики блоков питания/преобразователей': 'номинальные параметры при полной нагрузке', 'Вес': '950г', 'Рабочая температура': '-40...70°C', 'Количество выходов': '1', 'Электрическое подключение': 'клеммная колодка', 'Монтаж': 'открытое исполнение', 'Защита': 'от увеличения напряжения', 'Напряжение питания': '120...370В DC', 'КПД': '88%', 'Серия': 'HRP-300', 'Вид корпуса': '980A', 'Дополнительные функции': 'активное PFC', 'Выходное напряжение': '36В DC'}</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>www.tme.eu/Document/ee6f0e6a23c81f0c481af689425f21b2/INB-MN-ENCLOSED-RU.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>JSM-1618-20</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>JSM-1618-20</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Подшипник: опорная втулка; Øвнешн: 18мм; Øвнутр: 16мм; L: 20мм</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>0.0015</v>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>static.tme.eu/products_pics/b/6/7/b67f61bbcb1a038c229b06fb941a3f9d/421795.jpg</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>www.tme.eu/ru/details/jsm-1618-20/podshipniki-skolzheniia/igus/</t>
+        </is>
+      </c>
+      <c r="G46" s="3" t="inlineStr">
+        <is>
+          <t>{'Тип подшипника': 'опорная втулка', 'Внешний диаметр': '18мм', 'Внутренний диаметр': '16мм', 'Длина': '20мм', 'Материал': 'iglidur® J', 'Цвет': 'желтый', 'Характеристики механических элементов': 'бессмазочные', 'Рабочая температура': '-50...90°C', '#Common #name - #search': 'подшипник скольжения', 'Твердость по Шору': '74', 'Вид подшипника': 'скольжения'}</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>www.tme.eu/Document/86fbca866bb1e73a376a88d86a7e15e1/iglidur-J-EN.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>RK09K1130A8G</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>RK09K1130A8G</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Потенциометр: осевой; однооборотный,вертикальный; 10кОм; ±20%</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>0.00141</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>static.tme.eu/products_pics/6/d/6/6d6c777d2215a2471a47dc16a393bfe0/417706.jpg</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>www.tme.eu/ru/details/rk09k1130a8g/potentsiometry-odnooborotnye-ugolnye/alps/</t>
+        </is>
+      </c>
+      <c r="G47" s="3" t="inlineStr">
+        <is>
+          <t>{'Тип потенциометра': 'осевой', 'Вид потенциометра': 'однооборотный', 'Сопротивление': '10кОм', 'Погрешность': '±20%', 'Диаметр оси': '6мм', 'Длина оси': '7,4мм', 'Характеристика': 'линейная', 'Размеры корпуса': '9,8x11x6,8мм', 'Выводы': 'на печатную плату', 'Характеристики потенциометров': 'моно', 'Вид оси': 'с насечкой', 'Угол поворота механический': '300°', 'Шаг выводов': '2,54мм', 'Материал оси': 'пластик'}</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>www.tme.eu/Document/fb277d87df6cd625a5906cf03c82b793/ALPS_RK09K.PDF</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>P 128</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>P128</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Вилка; RJ12; PIN: 6; не экранированный; позолота; Конф: 6p6c; 26AWG</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>0.00086</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>static.tme.eu/products_pics/e/6/1/e61dc2845e5b5731bff8f9d8bc031d66/405307.jpg</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>www.tme.eu/ru/details/p128/razemy-rj/lumberg/p-128/</t>
+        </is>
+      </c>
+      <c r="G48" s="3" t="inlineStr">
+        <is>
+          <t>{'Разъем': 'вилка', 'Тип разъема': 'RJ12', 'Кол-во выводов': '6', 'Версия разъема': 'не экранированный', 'Покрытие контакта': 'позолота', 'Конфигурация выводов разъема': '6p6c', 'Электрический монтаж': 'IDC', 'Механический монтаж': 'на провод', 'Дополнительная информация': 'больше товаров данной серии доступно на www.tme.eu', 'Применяются с разъемами': 'плоский провод', 'Ресурс': '2000циклов', 'Размер провода': '26AWG'}</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>www.tme.eu/Document/f94641d56faeb499bf7a946683e7815c/P128.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="49"/>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
v 10, new database concept
</commit_message>
<xml_diff>
--- a/productdata.xlsx
+++ b/productdata.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="12645" windowWidth="22260" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="12585" windowWidth="22260" xWindow="0" yWindow="60"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -323,22 +323,22 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0" zoomScale="115" zoomScaleNormal="115">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -516,7 +516,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0.4637</v>
+        <v>0.4609</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -897,7 +897,7 @@
       </c>
       <c r="G15" s="3" t="inlineStr">
         <is>
-          <t>{'Тип диода': 'LED', 'Диаметр диода LED': '8мм', 'Исполнение диода LED': 'трехцветный', 'Цвет диодa LED': 'RGB', 'Длина волны красного цвета λd': '620...630нм', 'Длина волны зеленого цвета λd': '515...530нм', 'Длина волны голубого цвета': '465...475нм', 'Монтаж': 'THT', 'Характеристики диодов LED': 'программируемый', '#Common #name - #search': 'управляемый', 'Рабочая температура': '-25...80°C', 'Кол-во цветов': '16,7M', 'Рабочее напряжение': '1,8..2,2/2,8..3,1/2,9..3,2В'}</t>
+          <t>{'Тип диода': 'LED', 'Диаметр диода LED': '8мм', 'Исполнение диода LED': 'трехцветный', 'Цвет диодa LED': 'RGB', 'Длина волны красного цвета λd': '620...630нм', 'Длина волны зеленого цвета λd': '515...530нм', 'Длина волны голубого цвета': '465...475нм', 'Монтаж': 'THT', 'Характеристики диодов LED': 'программируемый', '#Common #name - #search': 'управляемый', 'Рабочая температура': '-25...80°C', 'Кол-во цветов': '16,7M', 'Рабочее напряжение': '1,8...2,2/2,8...3,1/2,9...3,2В'}</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -1090,7 +1090,7 @@
           <t>static.tme.eu/products_pics/b/5/0/b50d39ae95205c9cdb74ac3175ce020b/546968.jpg</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr">
+      <c r="F20" s="1" t="inlineStr">
         <is>
           <t>www.tme.eu/ru/details/m22-fled-rg/panelnye-aksessuary-standartnye/eaton-electric/</t>
         </is>
@@ -1447,7 +1447,7 @@
       </c>
       <c r="G29" s="3" t="inlineStr">
         <is>
-          <t>{'Тип микросхемы': 'микроконтроллер PIC', 'Память программы': '7кБ', 'Объем памяти SRAM': '256Б', 'Объем памяти EEPROM': '256Б', 'Интерфейс': 'MSSP (SPI / I2C)', 'Монтаж': 'SMD', 'Корпус': 'SO28', 'Кол-во входов/выходов': '25', 'Кол-во таймеров 8бит': '4', 'Кол-во таймеров 16бит': '1', 'Вид архитектуры': 'Harvard  8бит', 'Встроенный генератор': '32МГц', 'Семейство': 'PIC16', 'Рабочее напряжение': '1,8...5,5В'}</t>
+          <t>{'Тип микросхемы': 'микроконтроллер PIC', 'Память программы': '7кБ', 'Объем памяти SRAM': '256Б', 'Объем памяти EEPROM': '256Б', 'Интерфейс': 'MSSP (SPI / I2C)', 'Напряжение питания': '1,8...5,5В DC', 'Монтаж': 'SMD', 'Корпус': 'SO28', 'Кол-во входов/выходов': '25', 'Кол-во таймеров 8бит': '4', 'Кол-во таймеров 16бит': '1', 'Вид архитектуры': 'Harvard  8бит', 'Встроенный генератор': '32МГц', 'Семейство': 'PIC16'}</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
@@ -1760,7 +1760,7 @@
           <t>static.tme.eu/products_pics/0/c/e/0ceb1f77d747ee63f0513d0a22097555/213063.jpg</t>
         </is>
       </c>
-      <c r="F37" t="inlineStr">
+      <c r="F37" s="1" t="inlineStr">
         <is>
           <t>www.tme.eu/ru/details/ss49e/datchiki-kholla/honeywell/</t>
         </is>
@@ -1920,7 +1920,7 @@
           <t>static.tme.eu/products_pics/4/8/a/48a33ccfb5a851d5982dcdda0776f7ac/285338.jpg</t>
         </is>
       </c>
-      <c r="F41" t="inlineStr">
+      <c r="F41" s="1" t="inlineStr">
         <is>
           <t>www.tme.eu/ru/details/max660csa+/reguliatory-napriazheniia-mikroskhemy-dc-dc/maxim-integrated/</t>
         </is>
@@ -2216,8 +2216,52 @@
         </is>
       </c>
     </row>
-    <row r="49"/>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>PT10LV10103A2020S</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>PT10LV-10K</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Потенциометр: монтажный; однооборотный,горизонтальный; 10кОм</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>0.00062</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>static.tme.eu/products_pics/4/8/9/489b0853dca0e1de83ff0b390124fc9c/59967.jpg</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>www.tme.eu/ru/details/pt10lv-10k/potentsiometry-tht-odnooborotnye/piher/pt10lv10103a2020s/</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>{'Тип потенциометра': 'монтажный', 'Вид потенциометра': 'однооборотный', 'Сопротивление': '10кОм', 'Мощность': '150мВт', 'Погрешность': '±20%', 'Характеристика': 'линейная', 'Серия потенциометров': 'PT10LV', 'Стандарт потенциометра': '10мм', 'Угол поворота механический': '235 ±5°', 'Крутящий момент': '0,4...2Нсм', 'Рабочее напряжение макс.': '200В', 'Рабочая температура': '-25...70°C', 'Монтаж': 'THT', 'Шаг выводов': '5x10мм', 'Материал дорожки': 'углеродистый', 'Угол поворота электрический': '220 ±20°', 'Размеры корпуса': 'Ø10,3x4,5мм', 'Характеристики потенциометров': 'шлиц под крестовую отвертку'}</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>www.tme.eu/Document/0c37888a1f172cc56f5b3ed6f5607c24/PIHER_PT10_series.pdf</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F20" r:id="rId1"/>
+    <hyperlink ref="F37" r:id="rId2"/>
+    <hyperlink ref="F41" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>

</xml_diff>